<commit_message>
fixed change depth, added initialize to KPro_2016 for first point on KPRO Start
</commit_message>
<xml_diff>
--- a/templates/Fields for Excel sheets.xlsx
+++ b/templates/Fields for Excel sheets.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="70">
   <si>
     <t>Groundwater sheet</t>
   </si>
@@ -208,6 +208,24 @@
   </si>
   <si>
     <t>Salinity (% change)</t>
+  </si>
+  <si>
+    <t>Aux1</t>
+  </si>
+  <si>
+    <t>Aux2</t>
+  </si>
+  <si>
+    <t>U14</t>
+  </si>
+  <si>
+    <t>V14</t>
+  </si>
+  <si>
+    <t>Aux3</t>
+  </si>
+  <si>
+    <t>W14</t>
   </si>
 </sst>
 </file>
@@ -687,10 +705,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -842,6 +860,30 @@
       </c>
       <c r="B19" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>